<commit_message>
ECCE Makalesi Introduction ve References kısımları dışında tamamlandı aşağı yukarı. Yarın bu kısımları da ekleyip bugün yazdıklarımı tekrar düzenlemeyi düşünüyorum. Bu akşam vaktiniz olursa yazdığım kısımlara bakabilir misiniz? Yazdığım kısımda referansları henüz eklemediğim için herşey X olarak görünüyor ama kafamda aşağı yukarı hangi referansları vereceğim belli. @ozank @mesutto
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/GaN Model/AllDetailsIncluded/Results.xlsx
+++ b/Project/3501/Furkan/GaN Model/AllDetailsIncluded/Results.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>Vdc</t>
   </si>
@@ -157,6 +157,15 @@
   <si>
     <t>Eon + Eoff</t>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>ProdSim</t>
+  </si>
+  <si>
+    <t>ProdMeas</t>
+  </si>
 </sst>
 </file>
 
@@ -190,7 +199,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="26">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -329,6 +338,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -423,7 +444,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -458,9 +479,6 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="43" fontId="0" fillId="18" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -483,13 +501,7 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="22" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -498,7 +510,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="24" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -532,7 +552,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -626,7 +645,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -764,7 +782,6 @@
             <c:showLeaderLines val="0"/>
             <c:extLst>
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:layout/>
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
                   <c:spPr>
@@ -868,7 +885,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -989,7 +1005,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1064,7 +1079,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1441,7 +1455,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1562,7 +1575,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1637,7 +1649,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1962,7 +1973,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2083,7 +2093,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2158,7 +2167,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2524,6 +2532,13 @@
                   <a:rPr lang="tr-TR"/>
                   <a:t>Load Current</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="tr-TR" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t> (A)</a:t>
+                </a:r>
+                <a:endParaRPr lang="tr-TR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3089,6 +3104,13 @@
                   <a:rPr lang="tr-TR"/>
                   <a:t>Load Current</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="tr-TR" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t> (A)</a:t>
+                </a:r>
+                <a:endParaRPr lang="tr-TR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -3287,7 +3309,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -3612,6 +3634,58 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Prod Meas</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'ECCE Results'!$J$26:$J$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-EC4D-49D2-A429-1D74B6224DBC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -3623,6 +3697,70 @@
         <c:smooth val="0"/>
         <c:axId val="998524768"/>
         <c:axId val="998525184"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:v>Prod Sim</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'ECCE Results'!$J$20:$J$25</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>109</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>86</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>68</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>54</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>41</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>25</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-EC4D-49D2-A429-1D74B6224DBC}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="998524768"/>
@@ -3652,7 +3790,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="tr-TR"/>
-                  <a:t>Load Current</a:t>
+                  <a:t>Load Current (A)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4227,6 +4365,13 @@
                   <a:rPr lang="tr-TR"/>
                   <a:t>Load Current</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="tr-TR" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t> (A)</a:t>
+                </a:r>
+                <a:endParaRPr lang="tr-TR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -4792,6 +4937,13 @@
                   <a:rPr lang="tr-TR"/>
                   <a:t>Load Current</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="tr-TR" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t> (A)</a:t>
+                </a:r>
+                <a:endParaRPr lang="tr-TR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -5357,6 +5509,13 @@
                   <a:rPr lang="tr-TR"/>
                   <a:t>Load Current</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="tr-TR" sz="1000" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t> (A)</a:t>
+                </a:r>
+                <a:endParaRPr lang="tr-TR"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -11114,16 +11273,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>428625</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>532747</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>36918</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>230077</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>80579</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11144,16 +11303,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>152281</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:rowOff>45734</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11176,16 +11335,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>488146</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>323850</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>240195</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>83993</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11958,7 +12117,7 @@
         <v>0.61181555000000809</v>
       </c>
       <c r="K10">
-        <f>K2-J2</f>
+        <f t="shared" ref="K10:K15" si="1">K2-J2</f>
         <v>0.62000000000000011</v>
       </c>
       <c r="L10" s="20">
@@ -11974,35 +12133,35 @@
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="D11">
-        <f t="shared" ref="D11:D15" si="1">D3-B3</f>
+        <f t="shared" ref="D11:D15" si="2">D3-B3</f>
         <v>13.299999999999997</v>
       </c>
       <c r="E11">
-        <f t="shared" ref="E11:E15" si="2">100*D11/B3</f>
+        <f t="shared" ref="E11:E15" si="3">100*D11/B3</f>
         <v>53.199999999999989</v>
       </c>
       <c r="F11" s="12">
-        <f t="shared" ref="F11:F15" si="3">F3+G3</f>
+        <f t="shared" ref="F11:F15" si="4">F3+G3</f>
         <v>9.0819999999999999E-9</v>
       </c>
       <c r="H11" s="16">
-        <f t="shared" ref="H11:H14" si="4">ABS(I3-H3)*100/I3</f>
+        <f t="shared" ref="H11:H14" si="5">ABS(I3-H3)*100/I3</f>
         <v>7.6181615739840831</v>
       </c>
       <c r="I11" s="16">
-        <f t="shared" ref="I11:I15" si="5">ABS(I3-H3)*1000000</f>
+        <f t="shared" ref="I11:I15" si="6">ABS(I3-H3)*1000000</f>
         <v>6.1847883500000069</v>
       </c>
       <c r="K11">
-        <f>K3-J3</f>
+        <f t="shared" si="1"/>
         <v>0.71</v>
       </c>
       <c r="L11" s="20">
-        <f t="shared" ref="L11:L15" si="6">K3-L3</f>
+        <f t="shared" ref="L11:L15" si="7">K3-L3</f>
         <v>0.41999999999999993</v>
       </c>
       <c r="M11">
-        <f t="shared" ref="M11:M15" si="7">M3-J3</f>
+        <f t="shared" ref="M11:M15" si="8">M3-J3</f>
         <v>0.89000000000000012</v>
       </c>
     </row>
@@ -12010,35 +12169,35 @@
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="D12">
+        <f t="shared" si="2"/>
+        <v>14.700000000000003</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="3"/>
+        <v>73.500000000000014</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="4"/>
+        <v>7.1540000000000007E-9</v>
+      </c>
+      <c r="H12" s="16">
+        <f t="shared" si="5"/>
+        <v>1.3230287161056125</v>
+      </c>
+      <c r="I12" s="16">
+        <f t="shared" si="6"/>
+        <v>0.73742209999999586</v>
+      </c>
+      <c r="K12">
         <f t="shared" si="1"/>
-        <v>14.700000000000003</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="2"/>
-        <v>73.500000000000014</v>
-      </c>
-      <c r="F12" s="12">
-        <f t="shared" si="3"/>
-        <v>7.1540000000000007E-9</v>
-      </c>
-      <c r="H12" s="16">
-        <f t="shared" si="4"/>
-        <v>1.3230287161056125</v>
-      </c>
-      <c r="I12" s="16">
-        <f t="shared" si="5"/>
-        <v>0.73742209999999586</v>
-      </c>
-      <c r="K12">
-        <f>K4-J4</f>
         <v>0.74000000000000021</v>
       </c>
       <c r="L12" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.33999999999999986</v>
       </c>
       <c r="M12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.93000000000000016</v>
       </c>
     </row>
@@ -12049,35 +12208,35 @@
         <v>33</v>
       </c>
       <c r="D13">
+        <f t="shared" si="2"/>
+        <v>14.8</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="3"/>
+        <v>98.666666666666671</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="4"/>
+        <v>6.4740000000000006E-9</v>
+      </c>
+      <c r="H13" s="16">
+        <f t="shared" si="5"/>
+        <v>5.1105149769809453</v>
+      </c>
+      <c r="I13" s="16">
+        <f t="shared" si="6"/>
+        <v>2.0080223999999984</v>
+      </c>
+      <c r="K13">
         <f t="shared" si="1"/>
-        <v>14.8</v>
-      </c>
-      <c r="E13">
-        <f t="shared" si="2"/>
-        <v>98.666666666666671</v>
-      </c>
-      <c r="F13" s="12">
-        <f t="shared" si="3"/>
-        <v>6.4740000000000006E-9</v>
-      </c>
-      <c r="H13" s="16">
-        <f t="shared" si="4"/>
-        <v>5.1105149769809453</v>
-      </c>
-      <c r="I13" s="16">
-        <f t="shared" si="5"/>
-        <v>2.0080223999999984</v>
-      </c>
-      <c r="K13">
-        <f>K5-J5</f>
         <v>0.71999999999999975</v>
       </c>
       <c r="L13" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.5</v>
       </c>
       <c r="M13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.91999999999999993</v>
       </c>
     </row>
@@ -12087,35 +12246,35 @@
       </c>
       <c r="B14" s="4"/>
       <c r="D14">
+        <f t="shared" si="2"/>
+        <v>16.899999999999999</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="3"/>
+        <v>168.99999999999997</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="4"/>
+        <v>5.6770000000000001E-9</v>
+      </c>
+      <c r="H14" s="16">
+        <f t="shared" si="5"/>
+        <v>12.460112315715699</v>
+      </c>
+      <c r="I14" s="16">
+        <f t="shared" si="6"/>
+        <v>3.423591374999996</v>
+      </c>
+      <c r="K14">
         <f t="shared" si="1"/>
-        <v>16.899999999999999</v>
-      </c>
-      <c r="E14">
-        <f t="shared" si="2"/>
-        <v>168.99999999999997</v>
-      </c>
-      <c r="F14" s="12">
-        <f t="shared" si="3"/>
-        <v>5.6770000000000001E-9</v>
-      </c>
-      <c r="H14" s="16">
-        <f t="shared" si="4"/>
-        <v>12.460112315715699</v>
-      </c>
-      <c r="I14" s="16">
-        <f t="shared" si="5"/>
-        <v>3.423591374999996</v>
-      </c>
-      <c r="K14">
-        <f>K6-J6</f>
         <v>0.53000000000000025</v>
       </c>
       <c r="L14" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.29000000000000004</v>
       </c>
       <c r="M14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.93000000000000016</v>
       </c>
     </row>
@@ -12123,15 +12282,15 @@
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="D15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20.3</v>
       </c>
       <c r="E15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>406</v>
       </c>
       <c r="F15" s="12">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.2969999999999994E-9</v>
       </c>
       <c r="H15" s="16">
@@ -12139,19 +12298,19 @@
         <v>10.887938153920626</v>
       </c>
       <c r="I15" s="16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.2583391999999982</v>
       </c>
       <c r="K15">
-        <f>K7-J7</f>
+        <f t="shared" si="1"/>
         <v>0.58000000000000007</v>
       </c>
       <c r="L15" s="20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0.39000000000000012</v>
       </c>
       <c r="M15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>0.93000000000000016</v>
       </c>
     </row>
@@ -12238,7 +12397,7 @@
         <v>2.73</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" ref="E19:E23" si="8">1000000000000*(D19*0.000000001/C19)</f>
+        <f t="shared" ref="E19:E23" si="9">1000000000000*(D19*0.000000001/C19)</f>
         <v>237.39130434782612</v>
       </c>
     </row>
@@ -12256,7 +12415,7 @@
         <v>2.75</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>239.13043478260872</v>
       </c>
     </row>
@@ -12274,7 +12433,7 @@
         <v>3.13</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>272.17391304347831</v>
       </c>
     </row>
@@ -12292,7 +12451,7 @@
         <v>6.31</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>548.695652173913</v>
       </c>
     </row>
@@ -12310,7 +12469,7 @@
         <v>6.05</v>
       </c>
       <c r="E23" s="4">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>281.39534883720933</v>
       </c>
     </row>
@@ -12319,10 +12478,10 @@
       <c r="B24" s="4"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C27" s="32" t="s">
+      <c r="C27" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="D27" s="32"/>
+      <c r="D27" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -12506,641 +12665,887 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:X32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="33" t="s">
+      <c r="C1" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="D1" s="34" t="s">
+      <c r="D1" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="E1" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="F1" s="36" t="s">
+      <c r="F1" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="36" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="H1" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="I1" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="32" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="64">
+      <c r="A2" s="57">
         <v>1</v>
       </c>
-      <c r="B2" s="47">
+      <c r="B2" s="46">
         <v>400</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="46">
         <v>30</v>
       </c>
-      <c r="D2" s="48">
+      <c r="D2" s="47">
         <v>41</v>
       </c>
-      <c r="E2" s="49">
+      <c r="E2" s="48">
         <v>2.028</v>
       </c>
-      <c r="F2" s="50">
+      <c r="F2" s="49">
         <v>5.4020000000000001</v>
       </c>
-      <c r="G2" s="51">
+      <c r="G2" s="50">
         <v>10.7</v>
       </c>
-      <c r="H2" s="52">
+      <c r="H2" s="51">
         <v>2.6579999999999999</v>
       </c>
-      <c r="I2" s="69">
+      <c r="I2" s="62">
         <v>2.6579999999999999</v>
       </c>
-      <c r="J2" s="66">
+      <c r="J2" s="59">
         <f>D2 + G2</f>
         <v>51.7</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="65">
+      <c r="A3" s="58">
         <v>1</v>
       </c>
-      <c r="B3" s="54">
+      <c r="B3" s="53">
         <v>400</v>
       </c>
-      <c r="C3" s="54">
+      <c r="C3" s="53">
         <v>25</v>
       </c>
-      <c r="D3" s="40">
+      <c r="D3" s="39">
         <v>29.8</v>
       </c>
-      <c r="E3" s="41">
+      <c r="E3" s="40">
         <v>2.0710000000000002</v>
       </c>
-      <c r="F3" s="42">
+      <c r="F3" s="41">
         <v>3.99</v>
       </c>
-      <c r="G3" s="43">
+      <c r="G3" s="42">
         <v>10.3</v>
       </c>
-      <c r="H3" s="44">
+      <c r="H3" s="43">
         <v>2.7610000000000001</v>
       </c>
-      <c r="I3" s="45">
+      <c r="I3" s="44">
         <v>2.7610000000000001</v>
       </c>
-      <c r="J3" s="67">
+      <c r="J3" s="60">
         <f t="shared" ref="J3:J19" si="0">D3 + G3</f>
         <v>40.1</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="65">
+      <c r="A4" s="58">
         <v>1</v>
       </c>
-      <c r="B4" s="54">
+      <c r="B4" s="53">
         <v>400</v>
       </c>
-      <c r="C4" s="54">
+      <c r="C4" s="53">
         <v>20</v>
       </c>
-      <c r="D4" s="40">
+      <c r="D4" s="39">
         <v>22.2</v>
       </c>
-      <c r="E4" s="41">
+      <c r="E4" s="40">
         <v>1.944</v>
       </c>
-      <c r="F4" s="42">
+      <c r="F4" s="41">
         <v>3.6230000000000002</v>
       </c>
-      <c r="G4" s="43">
+      <c r="G4" s="42">
         <v>6.94</v>
       </c>
-      <c r="H4" s="44">
+      <c r="H4" s="43">
         <v>2.8260000000000001</v>
       </c>
-      <c r="I4" s="45">
+      <c r="I4" s="44">
         <v>2.8260000000000001</v>
       </c>
-      <c r="J4" s="67">
+      <c r="J4" s="60">
         <f t="shared" si="0"/>
         <v>29.14</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="65">
+      <c r="A5" s="58">
         <v>1</v>
       </c>
-      <c r="B5" s="54">
+      <c r="B5" s="53">
         <v>400</v>
       </c>
-      <c r="C5" s="54">
+      <c r="C5" s="53">
         <v>15</v>
       </c>
-      <c r="D5" s="40">
+      <c r="D5" s="39">
         <v>16.399999999999999</v>
       </c>
-      <c r="E5" s="41">
+      <c r="E5" s="40">
         <v>1.7669999999999999</v>
       </c>
-      <c r="F5" s="42">
+      <c r="F5" s="41">
         <v>2.91</v>
       </c>
-      <c r="G5" s="43">
+      <c r="G5" s="42">
         <v>6.98</v>
       </c>
-      <c r="H5" s="44">
+      <c r="H5" s="43">
         <v>4.5199999999999996</v>
       </c>
-      <c r="I5" s="45">
+      <c r="I5" s="44">
         <v>4.5199999999999996</v>
       </c>
-      <c r="J5" s="67">
+      <c r="J5" s="60">
         <f t="shared" si="0"/>
         <v>23.38</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="65">
+      <c r="A6" s="58">
         <v>1</v>
       </c>
-      <c r="B6" s="54">
+      <c r="B6" s="53">
         <v>400</v>
       </c>
-      <c r="C6" s="54">
+      <c r="C6" s="53">
         <v>10</v>
       </c>
-      <c r="D6" s="40">
+      <c r="D6" s="39">
         <v>11.9</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="40">
         <v>1.36</v>
       </c>
-      <c r="F6" s="42">
+      <c r="F6" s="41">
         <v>2.5099999999999998</v>
       </c>
-      <c r="G6" s="43">
+      <c r="G6" s="42">
         <v>5.79</v>
       </c>
-      <c r="H6" s="44">
+      <c r="H6" s="43">
         <v>6.2169999999999996</v>
       </c>
-      <c r="I6" s="45">
+      <c r="I6" s="44">
         <v>6.2169999999999996</v>
       </c>
-      <c r="J6" s="67">
+      <c r="J6" s="60">
         <f t="shared" si="0"/>
         <v>17.690000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="65">
+      <c r="A7" s="58">
         <v>1</v>
       </c>
-      <c r="B7" s="54">
+      <c r="B7" s="53">
         <v>400</v>
       </c>
-      <c r="C7" s="54">
+      <c r="C7" s="53">
         <v>5</v>
       </c>
-      <c r="D7" s="40">
+      <c r="D7" s="39">
         <v>8.36</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="40">
         <v>1.32</v>
       </c>
-      <c r="F7" s="42">
+      <c r="F7" s="41">
         <v>2.19</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="42">
         <v>6.13</v>
       </c>
-      <c r="H7" s="44">
+      <c r="H7" s="43">
         <v>10.6</v>
       </c>
-      <c r="I7" s="45">
+      <c r="I7" s="44">
         <v>10.6</v>
       </c>
-      <c r="J7" s="67">
+      <c r="J7" s="60">
         <f t="shared" si="0"/>
         <v>14.489999999999998</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="62">
+      <c r="A8" s="55">
         <v>2</v>
       </c>
-      <c r="B8" s="47">
+      <c r="B8" s="46">
         <v>400</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="46">
         <v>30</v>
       </c>
-      <c r="D8" s="48">
+      <c r="D8" s="47">
         <v>95.8</v>
       </c>
-      <c r="E8" s="49">
+      <c r="E8" s="48">
         <v>5.6139999999999999</v>
       </c>
-      <c r="F8" s="50">
+      <c r="F8" s="49">
         <v>8.3369999999999997</v>
       </c>
-      <c r="G8" s="51">
+      <c r="G8" s="50">
         <v>7.78</v>
       </c>
-      <c r="H8" s="52">
+      <c r="H8" s="51">
         <v>4.6550000000000002</v>
       </c>
-      <c r="I8" s="69">
+      <c r="I8" s="62">
         <v>4.6550000000000002</v>
       </c>
-      <c r="J8" s="66">
+      <c r="J8" s="59">
         <f t="shared" si="0"/>
         <v>103.58</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="63">
+      <c r="A9" s="56">
         <v>2</v>
       </c>
-      <c r="B9" s="54">
+      <c r="B9" s="53">
         <v>400</v>
       </c>
-      <c r="C9" s="54">
+      <c r="C9" s="53">
         <v>25</v>
       </c>
-      <c r="D9" s="40">
+      <c r="D9" s="39">
         <v>69.599999999999994</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="40">
         <v>4.9690000000000003</v>
       </c>
-      <c r="F9" s="42">
+      <c r="F9" s="41">
         <v>7.1779999999999999</v>
       </c>
-      <c r="G9" s="43">
+      <c r="G9" s="42">
         <v>7.95</v>
       </c>
-      <c r="H9" s="44">
+      <c r="H9" s="43">
         <v>5.8460000000000001</v>
       </c>
-      <c r="I9" s="45">
+      <c r="I9" s="44">
         <v>5.8460000000000001</v>
       </c>
-      <c r="J9" s="67">
+      <c r="J9" s="60">
         <f t="shared" si="0"/>
         <v>77.55</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="63">
+      <c r="A10" s="56">
         <v>2</v>
       </c>
-      <c r="B10" s="54">
+      <c r="B10" s="53">
         <v>400</v>
       </c>
-      <c r="C10" s="54">
+      <c r="C10" s="53">
         <v>20</v>
       </c>
-      <c r="D10" s="40">
+      <c r="D10" s="39">
         <v>52</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="40">
         <v>4.4779999999999998</v>
       </c>
-      <c r="F10" s="42">
+      <c r="F10" s="41">
         <v>5.6210000000000004</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="42">
         <v>7.73</v>
       </c>
-      <c r="H10" s="44">
+      <c r="H10" s="43">
         <v>6.798</v>
       </c>
-      <c r="I10" s="45">
+      <c r="I10" s="44">
         <v>6.7889999999999997</v>
       </c>
-      <c r="J10" s="67">
+      <c r="J10" s="60">
         <f t="shared" si="0"/>
         <v>59.730000000000004</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="63">
+      <c r="A11" s="56">
         <v>2</v>
       </c>
-      <c r="B11" s="54">
+      <c r="B11" s="53">
         <v>400</v>
       </c>
-      <c r="C11" s="54">
+      <c r="C11" s="53">
         <v>15</v>
       </c>
-      <c r="D11" s="40">
+      <c r="D11" s="39">
         <v>39.5</v>
       </c>
-      <c r="E11" s="41">
+      <c r="E11" s="40">
         <v>2.8580000000000001</v>
       </c>
-      <c r="F11" s="42">
+      <c r="F11" s="41">
         <v>4.6680000000000001</v>
       </c>
-      <c r="G11" s="43">
+      <c r="G11" s="42">
         <v>7.68</v>
       </c>
-      <c r="H11" s="44">
+      <c r="H11" s="43">
         <v>8.3879999999999999</v>
       </c>
-      <c r="I11" s="45">
+      <c r="I11" s="44">
         <v>8.3879999999999999</v>
       </c>
-      <c r="J11" s="67">
+      <c r="J11" s="60">
         <f t="shared" si="0"/>
         <v>47.18</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="63">
+      <c r="A12" s="56">
         <v>2</v>
       </c>
-      <c r="B12" s="54">
+      <c r="B12" s="53">
         <v>400</v>
       </c>
-      <c r="C12" s="54">
+      <c r="C12" s="53">
         <v>10</v>
       </c>
-      <c r="D12" s="40">
+      <c r="D12" s="39">
         <v>30.2</v>
       </c>
-      <c r="E12" s="41">
+      <c r="E12" s="40">
         <v>2.7280000000000002</v>
       </c>
-      <c r="F12" s="42">
+      <c r="F12" s="41">
         <v>3.91</v>
       </c>
-      <c r="G12" s="43">
+      <c r="G12" s="42">
         <v>7.23</v>
       </c>
-      <c r="H12" s="44">
+      <c r="H12" s="43">
         <v>11.74</v>
       </c>
-      <c r="I12" s="45">
+      <c r="I12" s="44">
         <v>11.74</v>
       </c>
-      <c r="J12" s="67">
+      <c r="J12" s="60">
         <f t="shared" si="0"/>
         <v>37.43</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="63">
+      <c r="A13" s="56">
         <v>2</v>
       </c>
-      <c r="B13" s="54">
+      <c r="B13" s="53">
         <v>400</v>
       </c>
-      <c r="C13" s="54">
+      <c r="C13" s="53">
         <v>5</v>
       </c>
-      <c r="D13" s="40">
+      <c r="D13" s="39">
         <v>22.8</v>
       </c>
-      <c r="E13" s="41">
+      <c r="E13" s="40">
         <v>2.4940000000000002</v>
       </c>
-      <c r="F13" s="42">
+      <c r="F13" s="41">
         <v>3.464</v>
       </c>
-      <c r="G13" s="43">
+      <c r="G13" s="42">
         <v>7.13</v>
       </c>
-      <c r="H13" s="44">
+      <c r="H13" s="43">
         <v>11.97</v>
       </c>
-      <c r="I13" s="45">
+      <c r="I13" s="44">
         <v>11.97</v>
       </c>
-      <c r="J13" s="67">
+      <c r="J13" s="60">
         <f t="shared" si="0"/>
         <v>29.93</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="46">
+      <c r="A14" s="45">
         <v>3</v>
       </c>
-      <c r="B14" s="47">
+      <c r="B14" s="46">
         <v>400</v>
       </c>
-      <c r="C14" s="47">
+      <c r="C14" s="46">
         <v>30</v>
       </c>
-      <c r="D14" s="48">
+      <c r="D14" s="47">
         <v>104.6</v>
       </c>
-      <c r="E14" s="49">
+      <c r="E14" s="48">
         <v>6.4550000000000001</v>
       </c>
-      <c r="F14" s="50">
+      <c r="F14" s="49">
         <v>9.1929999999999996</v>
       </c>
-      <c r="G14" s="51">
+      <c r="G14" s="50">
         <v>7.6</v>
       </c>
-      <c r="H14" s="52">
+      <c r="H14" s="51">
         <v>4.6079999999999997</v>
       </c>
-      <c r="I14" s="69">
+      <c r="I14" s="62">
         <v>4.6079999999999997</v>
       </c>
-      <c r="J14" s="66">
+      <c r="J14" s="59">
         <f t="shared" si="0"/>
         <v>112.19999999999999</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="53">
+      <c r="A15" s="52">
         <v>3</v>
       </c>
-      <c r="B15" s="54">
+      <c r="B15" s="53">
         <v>400</v>
       </c>
-      <c r="C15" s="54">
+      <c r="C15" s="53">
         <v>25</v>
       </c>
-      <c r="D15" s="40">
+      <c r="D15" s="39">
         <v>75</v>
       </c>
-      <c r="E15" s="41">
+      <c r="E15" s="40">
         <v>5.1929999999999996</v>
       </c>
-      <c r="F15" s="42">
+      <c r="F15" s="41">
         <v>8.5619999999999994</v>
       </c>
-      <c r="G15" s="43">
+      <c r="G15" s="42">
         <v>7.4</v>
       </c>
-      <c r="H15" s="44">
+      <c r="H15" s="43">
         <v>4.665</v>
       </c>
-      <c r="I15" s="45">
+      <c r="I15" s="44">
         <v>4.665</v>
       </c>
-      <c r="J15" s="67">
+      <c r="J15" s="60">
         <f t="shared" si="0"/>
         <v>82.4</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="53">
+      <c r="A16" s="52">
         <v>3</v>
       </c>
-      <c r="B16" s="54">
+      <c r="B16" s="53">
         <v>400</v>
       </c>
-      <c r="C16" s="54">
+      <c r="C16" s="53">
         <v>20</v>
       </c>
-      <c r="D16" s="40">
+      <c r="D16" s="39">
         <v>55.3</v>
       </c>
-      <c r="E16" s="41">
+      <c r="E16" s="40">
         <v>4.7640000000000002</v>
       </c>
-      <c r="F16" s="42">
+      <c r="F16" s="41">
         <v>5.835</v>
       </c>
-      <c r="G16" s="43">
+      <c r="G16" s="42">
         <v>7.13</v>
       </c>
-      <c r="H16" s="44">
+      <c r="H16" s="43">
         <v>6.7</v>
       </c>
-      <c r="I16" s="45">
+      <c r="I16" s="44">
         <v>6.7</v>
       </c>
-      <c r="J16" s="67">
+      <c r="J16" s="60">
         <f t="shared" si="0"/>
         <v>62.43</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="53">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A17" s="52">
         <v>3</v>
       </c>
-      <c r="B17" s="54">
+      <c r="B17" s="53">
         <v>400</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C17" s="53">
         <v>15</v>
       </c>
-      <c r="D17" s="40">
+      <c r="D17" s="39">
         <v>41.2</v>
       </c>
-      <c r="E17" s="41">
+      <c r="E17" s="40">
         <v>4.2249999999999996</v>
       </c>
-      <c r="F17" s="42">
+      <c r="F17" s="41">
         <v>5.149</v>
       </c>
-      <c r="G17" s="43">
+      <c r="G17" s="42">
         <v>7.07</v>
       </c>
-      <c r="H17" s="44">
+      <c r="H17" s="43">
         <v>6.9119999999999999</v>
       </c>
-      <c r="I17" s="45">
+      <c r="I17" s="44">
         <v>6.9119999999999999</v>
       </c>
-      <c r="J17" s="67">
+      <c r="J17" s="60">
         <f t="shared" si="0"/>
         <v>48.27</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="53">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A18" s="52">
         <v>3</v>
       </c>
-      <c r="B18" s="54">
+      <c r="B18" s="53">
         <v>400</v>
       </c>
-      <c r="C18" s="54">
+      <c r="C18" s="53">
         <v>10</v>
       </c>
-      <c r="D18" s="40">
+      <c r="D18" s="39">
         <v>31</v>
       </c>
-      <c r="E18" s="41">
+      <c r="E18" s="40">
         <v>2.3090000000000002</v>
       </c>
-      <c r="F18" s="42">
+      <c r="F18" s="41">
         <v>4.056</v>
       </c>
-      <c r="G18" s="43">
+      <c r="G18" s="42">
         <v>7.03</v>
       </c>
-      <c r="H18" s="44">
+      <c r="H18" s="43">
         <v>9.0120000000000005</v>
       </c>
-      <c r="I18" s="45">
+      <c r="I18" s="44">
         <v>9.0120000000000005</v>
       </c>
-      <c r="J18" s="67">
+      <c r="J18" s="60">
         <f t="shared" si="0"/>
         <v>38.03</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="55">
+    <row r="19" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="52">
         <v>3</v>
       </c>
-      <c r="B19" s="56">
+      <c r="B19" s="53">
         <v>400</v>
       </c>
-      <c r="C19" s="56">
+      <c r="C19" s="53">
         <v>5</v>
       </c>
-      <c r="D19" s="57">
+      <c r="D19" s="39">
         <v>23.1</v>
       </c>
-      <c r="E19" s="58">
+      <c r="E19" s="40">
         <v>2.214</v>
       </c>
-      <c r="F19" s="59">
+      <c r="F19" s="41">
         <v>3.5470000000000002</v>
       </c>
-      <c r="G19" s="60">
+      <c r="G19" s="42">
         <v>7.02</v>
       </c>
-      <c r="H19" s="61">
+      <c r="H19" s="43">
         <v>12.2</v>
       </c>
-      <c r="I19" s="70">
+      <c r="I19" s="44">
         <v>12.2</v>
       </c>
-      <c r="J19" s="68">
+      <c r="J19" s="60">
         <f t="shared" si="0"/>
         <v>30.12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A20" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="B20" s="46">
+        <v>400</v>
+      </c>
+      <c r="C20" s="46">
+        <v>30</v>
+      </c>
+      <c r="D20" s="46"/>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="59">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A21" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="B21" s="53">
+        <v>400</v>
+      </c>
+      <c r="C21" s="53">
+        <v>25</v>
+      </c>
+      <c r="D21" s="53"/>
+      <c r="E21" s="53"/>
+      <c r="F21" s="53"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="53"/>
+      <c r="I21" s="53"/>
+      <c r="J21" s="60">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A22" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="53">
+        <v>400</v>
+      </c>
+      <c r="C22" s="53">
+        <v>20</v>
+      </c>
+      <c r="D22" s="53"/>
+      <c r="E22" s="53"/>
+      <c r="F22" s="53"/>
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="60">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A23" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="53">
+        <v>400</v>
+      </c>
+      <c r="C23" s="53">
+        <v>15</v>
+      </c>
+      <c r="D23" s="53"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="53"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="60">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="53">
+        <v>400</v>
+      </c>
+      <c r="C24" s="53">
+        <v>10</v>
+      </c>
+      <c r="D24" s="53"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="53"/>
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="60">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="54">
+        <v>400</v>
+      </c>
+      <c r="C25" s="54">
+        <v>5</v>
+      </c>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="F25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="61">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A26" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="46">
+        <v>400</v>
+      </c>
+      <c r="C26" s="46">
+        <v>30</v>
+      </c>
+      <c r="D26" s="46"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="59">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="B27" s="53">
+        <v>400</v>
+      </c>
+      <c r="C27" s="53">
+        <v>25</v>
+      </c>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
+      <c r="F27" s="53"/>
+      <c r="G27" s="53"/>
+      <c r="H27" s="53"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="60">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="B28" s="53">
+        <v>400</v>
+      </c>
+      <c r="C28" s="53">
+        <v>20</v>
+      </c>
+      <c r="D28" s="53"/>
+      <c r="E28" s="53"/>
+      <c r="F28" s="53"/>
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="60">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="53">
+        <v>400</v>
+      </c>
+      <c r="C29" s="53">
+        <v>15</v>
+      </c>
+      <c r="D29" s="53"/>
+      <c r="E29" s="53"/>
+      <c r="F29" s="53"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="53"/>
+      <c r="I29" s="53"/>
+      <c r="J29" s="60">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" s="66" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" s="53">
+        <v>400</v>
+      </c>
+      <c r="C30" s="53">
+        <v>10</v>
+      </c>
+      <c r="D30" s="53"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="60">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="68" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="54">
+        <v>400</v>
+      </c>
+      <c r="C31" s="54">
+        <v>5</v>
+      </c>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+      <c r="F31" s="54"/>
+      <c r="G31" s="54"/>
+      <c r="H31" s="54"/>
+      <c r="I31" s="54"/>
+      <c r="J31" s="61">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X32" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
The article is reviewed in the consideration of revision notes of @mesutto .
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/GaN Model/AllDetailsIncluded/Results.xlsx
+++ b/Project/3501/Furkan/GaN Model/AllDetailsIncluded/Results.xlsx
@@ -2542,7 +2542,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2663,7 +2662,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2738,7 +2736,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4375,7 +4372,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4496,7 +4492,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -4571,7 +4566,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4947,7 +4941,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5068,7 +5061,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5143,7 +5135,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5519,7 +5510,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5648,7 +5638,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -5723,7 +5712,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12667,8 +12655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14:F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>